<commit_message>
Tweak calcs, update input.
Group SEGES digestate values correctly now.
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/lit_summary/data/literature.xlsx
+++ b/2021-0313846_slurry_separation/lit_summary/data/literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au583430\OneDrive - Aarhus Universitet\Dokumenter\Myndighedsbetjening\2021-0313846 Vurdering af separation\shared folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3140" documentId="13_ncr:1_{3B150B77-9D6B-4B7E-8519-03CDD6C3F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EE98370-263B-485B-A8E4-2463896733FF}"/>
+  <xr:revisionPtr revIDLastSave="3142" documentId="13_ncr:1_{3B150B77-9D6B-4B7E-8519-03CDD6C3F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C44132F-E5A9-4479-8BA9-6BE4441B6787}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3045" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="521">
   <si>
     <t>paper</t>
   </si>
@@ -2846,10 +2846,7 @@
     <t>screw press + decanting centrifuge</t>
   </si>
   <si>
-    <t>7. NE Videbæk</t>
-  </si>
-  <si>
-    <t>8. NE Videbæk</t>
+    <t>NE Videbæk</t>
   </si>
   <si>
     <t>DM%</t>
@@ -3134,7 +3131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3325,7 +3322,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Beregning" xfId="1" builtinId="22"/>
@@ -3994,8 +3990,8 @@
   <dimension ref="A1:BF211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="11" ySplit="3" topLeftCell="O98" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I110" sqref="I110"/>
+      <pane xSplit="11" ySplit="3" topLeftCell="O198" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="V207" sqref="V207"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
     </sheetView>
@@ -22543,7 +22539,7 @@
       <c r="H190" t="s">
         <v>486</v>
       </c>
-      <c r="I190" s="82" t="s">
+      <c r="I190" t="s">
         <v>285</v>
       </c>
       <c r="J190" s="19" t="s">
@@ -22613,7 +22609,7 @@
       <c r="H191" t="s">
         <v>486</v>
       </c>
-      <c r="I191" s="82" t="s">
+      <c r="I191" t="s">
         <v>285</v>
       </c>
       <c r="J191" s="19" t="s">
@@ -22680,7 +22676,7 @@
       <c r="F192" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="I192" s="82" t="s">
+      <c r="I192" t="s">
         <v>285</v>
       </c>
       <c r="J192" s="19" t="s">
@@ -22728,7 +22724,7 @@
       <c r="H193" t="s">
         <v>486</v>
       </c>
-      <c r="I193" s="82" t="s">
+      <c r="I193" t="s">
         <v>285</v>
       </c>
       <c r="J193" s="19" t="s">
@@ -22782,7 +22778,7 @@
       <c r="H194" t="s">
         <v>486</v>
       </c>
-      <c r="I194" s="82" t="s">
+      <c r="I194" t="s">
         <v>285</v>
       </c>
       <c r="J194" s="19" t="s">
@@ -22833,7 +22829,7 @@
       <c r="F195" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="I195" s="82" t="s">
+      <c r="I195" t="s">
         <v>285</v>
       </c>
       <c r="K195" s="20" t="s">
@@ -23491,7 +23487,7 @@
         <v>4.7</v>
       </c>
       <c r="V206" s="19" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="207" spans="1:47">
@@ -23552,18 +23548,18 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="B2" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -23576,10 +23572,10 @@
     <row r="3" spans="1:7">
       <c r="B3" s="3"/>
       <c r="F3" t="s">
+        <v>512</v>
+      </c>
+      <c r="G3" t="s">
         <v>513</v>
-      </c>
-      <c r="G3" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -23656,7 +23652,7 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B8" s="13">
         <f>(B4-B6)/(B5-B6)</f>
@@ -23685,13 +23681,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C10" t="s">
         <v>516</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>517</v>
-      </c>
-      <c r="E10" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -23714,17 +23710,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -23962,12 +23958,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -23976,14 +23966,20 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A662E54A-967B-44BB-90F9-1599E728B1A7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A402CE-7A4B-44ED-A208-3884D1FBDB29}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DF2204-8892-4A94-90A5-6DCDBF4AC498}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A402CE-7A4B-44ED-A208-3884D1FBDB29}"/>
 </file>
</xml_diff>

<commit_message>
Group by set, add small table export
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/lit_summary/data/literature.xlsx
+++ b/2021-0313846_slurry_separation/lit_summary/data/literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au583430\OneDrive - Aarhus Universitet\Dokumenter\Myndighedsbetjening\2021-0313846 Vurdering af separation\shared folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3142" documentId="13_ncr:1_{3B150B77-9D6B-4B7E-8519-03CDD6C3F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C44132F-E5A9-4479-8BA9-6BE4441B6787}"/>
+  <xr:revisionPtr revIDLastSave="3175" documentId="13_ncr:1_{3B150B77-9D6B-4B7E-8519-03CDD6C3F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{796A2826-0943-4F4D-A3C5-0727FFBC982F}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3045" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3990,8 +3990,8 @@
   <dimension ref="A1:BF211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="11" ySplit="3" topLeftCell="O198" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="V207" sqref="V207"/>
+      <pane xSplit="11" ySplit="3" topLeftCell="W192" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AD207" sqref="AD207"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
     </sheetView>
@@ -4881,6 +4881,9 @@
       <c r="Z8" s="18" t="s">
         <v>179</v>
       </c>
+      <c r="AD8" s="7">
+        <v>1</v>
+      </c>
       <c r="AO8" s="32"/>
     </row>
     <row r="9" spans="1:48" ht="15" customHeight="1">
@@ -7317,6 +7320,9 @@
       <c r="AC35" s="20">
         <v>3.3</v>
       </c>
+      <c r="AD35" s="7">
+        <v>1</v>
+      </c>
       <c r="AE35" t="s">
         <v>189</v>
       </c>
@@ -7606,6 +7612,9 @@
       <c r="AC38" s="20">
         <v>2.5</v>
       </c>
+      <c r="AD38" s="7">
+        <v>2</v>
+      </c>
       <c r="AE38" t="s">
         <v>189</v>
       </c>
@@ -7890,6 +7899,9 @@
       <c r="AC41" s="20">
         <v>1.8</v>
       </c>
+      <c r="AD41" s="7">
+        <v>1</v>
+      </c>
       <c r="AE41" t="s">
         <v>189</v>
       </c>
@@ -8172,6 +8184,9 @@
       </c>
       <c r="AC44" s="20">
         <v>1.4</v>
+      </c>
+      <c r="AD44" s="7">
+        <v>2</v>
       </c>
       <c r="AE44" t="s">
         <v>189</v>
@@ -10928,7 +10943,9 @@
       <c r="AC71" s="20">
         <v>0.2</v>
       </c>
-      <c r="AD71" s="17"/>
+      <c r="AD71" s="17">
+        <v>1</v>
+      </c>
       <c r="AE71" t="s">
         <v>189</v>
       </c>
@@ -11180,7 +11197,9 @@
       <c r="AC73" s="20">
         <v>2.5</v>
       </c>
-      <c r="AD73" s="17"/>
+      <c r="AD73" s="17">
+        <v>1</v>
+      </c>
       <c r="AE73" t="s">
         <v>189</v>
       </c>
@@ -11569,7 +11588,9 @@
       <c r="AC76" s="20">
         <v>1.9</v>
       </c>
-      <c r="AD76" s="17"/>
+      <c r="AD76" s="17">
+        <v>2</v>
+      </c>
       <c r="AE76" t="s">
         <v>189</v>
       </c>
@@ -14495,7 +14516,9 @@
       <c r="AA105" s="67"/>
       <c r="AB105" s="54"/>
       <c r="AC105" s="54"/>
-      <c r="AD105" s="55"/>
+      <c r="AD105" s="55">
+        <v>1</v>
+      </c>
       <c r="AE105" s="56"/>
       <c r="AF105" s="55"/>
       <c r="AG105" s="56"/>
@@ -22516,6 +22539,9 @@
       <c r="Y189" s="20" t="s">
         <v>157</v>
       </c>
+      <c r="AD189" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="190" spans="1:47">
       <c r="A190" s="63" t="s">
@@ -22586,6 +22612,9 @@
       <c r="Y190" s="20" t="s">
         <v>168</v>
       </c>
+      <c r="AD190" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="191" spans="1:47">
       <c r="A191" s="63" t="s">
@@ -22655,6 +22684,9 @@
       </c>
       <c r="Y191" s="20" t="s">
         <v>186</v>
+      </c>
+      <c r="AD191" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:47">
@@ -22701,6 +22733,9 @@
         <v>488</v>
       </c>
       <c r="X192" s="64"/>
+      <c r="AD192" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="193" spans="1:47">
       <c r="A193" s="63" t="s">
@@ -22755,6 +22790,9 @@
         <v>488</v>
       </c>
       <c r="X193" s="64"/>
+      <c r="AD193" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="194" spans="1:47">
       <c r="A194" s="63" t="s">
@@ -22809,6 +22847,9 @@
         <v>488</v>
       </c>
       <c r="X194" s="64"/>
+      <c r="AD194" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="195" spans="1:47" ht="30">
       <c r="A195" s="3" t="s">
@@ -22864,6 +22905,9 @@
       <c r="X195" s="70" t="s">
         <v>494</v>
       </c>
+      <c r="AD195" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="196" spans="1:47" ht="30">
       <c r="A196" s="3" t="s">
@@ -22933,6 +22977,9 @@
       <c r="X196" s="70" t="s">
         <v>494</v>
       </c>
+      <c r="AD196" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="1:47" ht="30">
       <c r="A197" s="3" t="s">
@@ -23002,6 +23049,9 @@
       <c r="X197" s="70" t="s">
         <v>494</v>
       </c>
+      <c r="AD197" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="198" spans="1:47" ht="30">
       <c r="A198" s="3" t="s">
@@ -23053,6 +23103,9 @@
       <c r="U198" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD198" s="7">
+        <v>0</v>
+      </c>
       <c r="AU198" t="s">
         <v>503</v>
       </c>
@@ -23107,6 +23160,9 @@
       <c r="U199" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD199" s="7">
+        <v>1</v>
+      </c>
       <c r="AU199" t="s">
         <v>503</v>
       </c>
@@ -23176,6 +23232,9 @@
       <c r="U200" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD200" s="7">
+        <v>1</v>
+      </c>
       <c r="AU200" t="s">
         <v>503</v>
       </c>
@@ -23245,6 +23304,9 @@
       <c r="U201" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD201" s="7">
+        <v>1</v>
+      </c>
       <c r="AU201" t="s">
         <v>503</v>
       </c>
@@ -23299,6 +23361,9 @@
       <c r="U202" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD202" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="203" spans="1:47" ht="30">
       <c r="A203" s="3" t="s">
@@ -23365,6 +23430,9 @@
       <c r="U203" s="19" t="s">
         <v>502</v>
       </c>
+      <c r="AD203" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="204" spans="1:47" ht="30">
       <c r="A204" s="3" t="s">
@@ -23430,6 +23498,9 @@
       </c>
       <c r="U204" s="19" t="s">
         <v>502</v>
+      </c>
+      <c r="AD204" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:47">
@@ -23460,6 +23531,9 @@
       <c r="V205" s="19" t="s">
         <v>508</v>
       </c>
+      <c r="AD205" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="206" spans="1:47">
       <c r="A206" s="3" t="s">
@@ -23488,6 +23562,9 @@
       </c>
       <c r="V206" s="19" t="s">
         <v>508</v>
+      </c>
+      <c r="AD206" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:47">
@@ -23729,6 +23806,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000AF577DD6E8D684CAFF1362865632EC1" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="124ec2e8304c3c5bf89d682421b875f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2f148fa0-8849-43ca-a1ad-3219566f6285" xmlns:ns4="3b7cc9eb-1f2c-44c2-aef1-68ff51cd8f88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="464bcc6cf6fa934ceccd475991ae2ccb" ns3:_="" ns4:_="">
     <xsd:import namespace="2f148fa0-8849-43ca-a1ad-3219566f6285"/>
@@ -23957,23 +24049,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A662E54A-967B-44BB-90F9-1599E728B1A7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A402CE-7A4B-44ED-A208-3884D1FBDB29}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23981,5 +24058,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A402CE-7A4B-44ED-A208-3884D1FBDB29}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A662E54A-967B-44BB-90F9-1599E728B1A7}"/>
 </file>
</xml_diff>